<commit_message>
[product-importing] Fixed all broken tests
</commit_message>
<xml_diff>
--- a/app/tests/assets/lixeirasAlgumasErradas.xlsx
+++ b/app/tests/assets/lixeirasAlgumasErradas.xlsx
@@ -103,7 +103,7 @@
     <t>Lixeira sem LM</t>
   </si>
   <si>
-    <t>4af9f23d8ead0e1d32000008</t>
+    <t>lixeiras</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
   <dimension ref="A2:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>